<commit_message>
Add: add validation in frontend
</commit_message>
<xml_diff>
--- a/backend/.backup/data_tamu.xlsx
+++ b/backend/.backup/data_tamu.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -622,9 +622,229 @@
         <v>Keluarga Mempelai Pria</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D12" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D13" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D14" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D15" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D16" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D17" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D18" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D19" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D20" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Keluarga Mempelai Wanita</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D21" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" t="str">
+        <v>Keluarga Mempelai Wanita</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D22" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Keluarga Mempelai Wanita</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: build controller for route
</commit_message>
<xml_diff>
--- a/backend/.backup/data_tamu.xlsx
+++ b/backend/.backup/data_tamu.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -842,9 +842,29 @@
         <v>Keluarga Mempelai Wanita</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>DDMMYYFN20</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Fahrezi Rizqiawan</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Kota Bekasi</v>
+      </c>
+      <c r="D23" t="str">
+        <v>089662690020</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Kerabat Mempelai Pria</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>